<commit_message>
value now from raw obk files
</commit_message>
<xml_diff>
--- a/oakbrook_monitoring_sheet.xlsx
+++ b/oakbrook_monitoring_sheet.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B244"/>
+  <dimension ref="A1:B249"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9967794.360000003</v>
+        <v>16680771.75</v>
       </c>
     </row>
     <row r="4">
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9967794.360000003</v>
+        <v>10137542.28</v>
       </c>
     </row>
     <row r="5">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>6543229.47</v>
       </c>
     </row>
     <row r="6">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>213537280.4900002</v>
+        <v>213537280.49</v>
       </c>
     </row>
     <row r="9">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>104691701.6399999</v>
+        <v>104691701.64</v>
       </c>
     </row>
     <row r="10">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>108845578.8500002</v>
+        <v>108845578.85</v>
       </c>
     </row>
     <row r="11">
@@ -626,175 +626,179 @@
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>Financial &amp; Performance Covenants</t>
+          <t>WA APR</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>Financial Covenants</t>
-        </is>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>77.04150334380085</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>TNW</t>
-        </is>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ares</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>53.30653799205933</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>30989072.96</v>
+        <v>23.73496535174152</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>30989072.96</v>
-      </c>
+      <c r="A28" s="2" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
+          <t>Financial &amp; Performance Covenants</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Financial Covenants</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>TNW</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>30989072.96</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Threshold</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>30989072.96</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
           <t>Operational Liquidity</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
         <v>5827071.87</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>Performance Covenants (rolling 3m avg)</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>Excess spread</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>27.12%</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>Blended delinquencies</t>
-        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>4.84%</t>
-        </is>
+          <t>Threshold</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>2000000</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>Blended losses</t>
+          <t>Performance Covenants (rolling 3m avg)</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>23.28%</t>
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>Excess spread</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="inlineStr">
-        <is>
-          <t>First Payment Default</t>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>27.12%</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>3.14%</t>
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>Blended delinquencies</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="inlineStr"/>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>4.84%</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>Concentration Limits</t>
+          <t>Blended losses</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="inlineStr">
-        <is>
-          <t>Concentration Limits</t>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>23.28%</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>WA Original Term</t>
+          <t>First Payment Default</t>
         </is>
       </c>
     </row>
@@ -804,1991 +808,2027 @@
           <t>Actuals</t>
         </is>
       </c>
-      <c r="B45" t="n">
-        <v>29.09695207244295</v>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>3.14%</t>
+        </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>36</v>
-      </c>
+      <c r="A46" s="2" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>WA Delphi Score</t>
+          <t>Concentration Limits</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>736.4361319937702</v>
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>Concentration Limits</t>
+        </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>700</v>
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>WA Original Term</t>
+        </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="inlineStr">
-        <is>
-          <t>Average Advance</t>
-        </is>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>29.09695207244295</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2252.317491142003</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>WA Delphi Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>736.4361319937702</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
         <is>
           <t>Threshold</t>
         </is>
       </c>
-      <c r="B52" t="n">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="2" t="inlineStr">
-        <is>
-          <t>Concentration Limits</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="2" t="inlineStr">
-        <is>
-          <t>Original term &gt;48</t>
-        </is>
+      <c r="B54" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>6.16%</t>
+      <c r="A55" s="2" t="inlineStr">
+        <is>
+          <t>Average Advance</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>2252.317491142003</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
           <t>Threshold</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="2" t="inlineStr">
-        <is>
-          <t>Near-Prime &amp; Delphi score &lt; 725</t>
-        </is>
+      <c r="B57" t="n">
+        <v>3600</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>14.37%</t>
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>Concentration Limits</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>22.50%</t>
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>Original term &gt;48</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="inlineStr">
-        <is>
-          <t>Near-Prime &amp; Delphi score of &lt; 650</t>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>6.16%</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4.59%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>10.00%</t>
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>Near-Prime &amp; Delphi score &lt; 725</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="inlineStr">
-        <is>
-          <t>Original UPB &gt; £5,000</t>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>14.37%</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>4.90%</t>
+          <t>22.50%</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>25.00%</t>
+      <c r="A65" s="2" t="inlineStr">
+        <is>
+          <t>Near-Prime &amp; Delphi score of &lt; 650</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="inlineStr">
-        <is>
-          <t>Non-Prime &amp; Delphi Score of &lt; 500</t>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>4.59%</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>11.64%</t>
+          <t>10.00%</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>12.50%</t>
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>Original UPB &gt; £5,000</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="inlineStr">
-        <is>
-          <t>Receivables in arrears (1-30DPD)</t>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>4.90%</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>3.51%</t>
+          <t>25.00%</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>8.00%</t>
+      <c r="A71" s="2" t="inlineStr">
+        <is>
+          <t>Non-Prime &amp; Delphi Score of &lt; 500</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="inlineStr">
-        <is>
-          <t>Reperformed Covid-19 Modified</t>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>11.64%</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>0.01%</t>
+          <t>12.50%</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>15.00%</t>
+      <c r="A74" s="2" t="inlineStr">
+        <is>
+          <t>Receivables in arrears (1-30DPD)</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="inlineStr">
-        <is>
-          <t>Reperformed Covid-19 Modified (Total Holiday &gt;3m)</t>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>3.51%</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
+          <t>8.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="inlineStr">
+        <is>
+          <t>Reperformed Covid-19 Modified</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
           <t>0.01%</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>5.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="2" t="inlineStr">
-        <is>
-          <t>Prime &amp; Delphi score of &lt; 700</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>15.00%</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>10.00%</t>
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>Reperformed Covid-19 Modified (Total Holiday &gt;3m)</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="inlineStr">
-        <is>
-          <t>Prime Receivables %</t>
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>0.01%</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>0.03%</t>
+          <t>5.00%</t>
         </is>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>10.00%</t>
+      <c r="A83" s="2" t="inlineStr">
+        <is>
+          <t>Prime &amp; Delphi score of &lt; 700</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="inlineStr">
-        <is>
-          <t>Thin File Receivable %</t>
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>10.00%</t>
         </is>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>5.00%</t>
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>Prime Receivables %</t>
         </is>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="inlineStr">
-        <is>
-          <t>Single Borrower &gt; £10k/ Single Large Loan Borrower &gt; £15k</t>
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>0.03%</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Threshold</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
+          <t>10.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="inlineStr">
+        <is>
+          <t>Thin File Receivable %</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
           <t>0.00%</t>
         </is>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
+    <row r="91">
+      <c r="A91" t="inlineStr">
         <is>
           <t>Threshold</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="2" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="2" t="inlineStr">
-        <is>
-          <t>Back Book and Front Book</t>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>5.00%</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="inlineStr">
         <is>
+          <t>Single Borrower &gt; £10k/ Single Large Loan Borrower &gt; £15k</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Threshold</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>Back Book and Front Book</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="inlineStr">
+        <is>
           <t>Cumulative Defaults</t>
         </is>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="2" t="inlineStr">
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
         <is>
           <t>Back Book Non Prime Cumulative Defaults</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="2" t="inlineStr">
-        <is>
-          <t>Cohort</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="2" t="inlineStr">
-        <is>
-          <t>2017 Q1</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>23.63%</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>Tier 1 Threshold</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>30.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>Tier 2 Threshold</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>35.00%</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>2017 Q2</t>
+          <t>Cohort</t>
         </is>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>22.25%</t>
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>2017 Q1</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>23.63%</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" s="2" t="inlineStr">
-        <is>
-          <t>2017 Q3</t>
-        </is>
-      </c>
-    </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>22.67%</t>
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>2017 Q2</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>22.25%</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" s="2" t="inlineStr">
-        <is>
-          <t>2017 Q4</t>
-        </is>
-      </c>
-    </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>22.91%</t>
+      <c r="A108" s="2" t="inlineStr">
+        <is>
+          <t>2017 Q3</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>22.67%</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" s="2" t="inlineStr">
-        <is>
-          <t>2018 Q1</t>
-        </is>
-      </c>
-    </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>22.23%</t>
+      <c r="A112" s="2" t="inlineStr">
+        <is>
+          <t>2017 Q4</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>22.91%</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" s="2" t="inlineStr">
-        <is>
-          <t>2018 Q2</t>
-        </is>
-      </c>
-    </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>21.25%</t>
+      <c r="A116" s="2" t="inlineStr">
+        <is>
+          <t>2018 Q1</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>22.23%</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" s="2" t="inlineStr">
-        <is>
-          <t>2018 Q3</t>
-        </is>
-      </c>
-    </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>20.97%</t>
+      <c r="A120" s="2" t="inlineStr">
+        <is>
+          <t>2018 Q2</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>21.25%</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" s="2" t="inlineStr">
-        <is>
-          <t>2018 Q4</t>
-        </is>
-      </c>
-    </row>
     <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>21.93%</t>
+      <c r="A124" s="2" t="inlineStr">
+        <is>
+          <t>2018 Q3</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>20.97%</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" s="2" t="inlineStr">
-        <is>
-          <t>2019 Q1</t>
-        </is>
-      </c>
-    </row>
     <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>22.14%</t>
+      <c r="A128" s="2" t="inlineStr">
+        <is>
+          <t>2018 Q4</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>21.93%</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" s="2" t="inlineStr">
-        <is>
-          <t>2019 Q2</t>
-        </is>
-      </c>
-    </row>
     <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>21.62%</t>
+      <c r="A132" s="2" t="inlineStr">
+        <is>
+          <t>2019 Q1</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>22.14%</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" s="2" t="inlineStr">
-        <is>
-          <t>2019 Q3</t>
-        </is>
-      </c>
-    </row>
     <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>21.48%</t>
+      <c r="A136" s="2" t="inlineStr">
+        <is>
+          <t>2019 Q2</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>21.62%</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" s="2" t="inlineStr">
-        <is>
-          <t>2019 Q4</t>
-        </is>
-      </c>
-    </row>
     <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>21.68%</t>
+      <c r="A140" s="2" t="inlineStr">
+        <is>
+          <t>2019 Q3</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>21.48%</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
     </row>
-    <row r="143">
-      <c r="A143" s="2" t="inlineStr">
+    <row r="144">
+      <c r="A144" s="2" t="inlineStr">
+        <is>
+          <t>2019 Q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>21.68%</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Tier 1 Threshold</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>35.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="inlineStr">
         <is>
           <t>2020 Q1</t>
         </is>
       </c>
     </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
         <is>
           <t>18.55%</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="2" t="inlineStr">
-        <is>
-          <t>Tier 1 Threshold</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="2" t="inlineStr">
-        <is>
-          <t>Tier 2 Threshold</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="2" t="inlineStr">
-        <is>
-          <t>2020 Q3</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>17.39%</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" s="2" t="inlineStr">
-        <is>
-          <t>Tier 1 Threshold</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>2020 Q4</t>
+          <t>Tier 2 Threshold</t>
         </is>
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>16.78%</t>
+      <c r="A152" s="2" t="inlineStr">
+        <is>
+          <t>2020 Q3</t>
         </is>
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="2" t="inlineStr">
-        <is>
-          <t>Tier 1 Threshold</t>
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>17.39%</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>2021 Q1</t>
+          <t>Tier 2 Threshold</t>
         </is>
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>23.53%</t>
+      <c r="A156" s="2" t="inlineStr">
+        <is>
+          <t>2020 Q4</t>
         </is>
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="2" t="inlineStr">
-        <is>
-          <t>Tier 1 Threshold</t>
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>16.78%</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>2021 Q2</t>
+          <t>Tier 2 Threshold</t>
         </is>
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>25.08%</t>
+      <c r="A160" s="2" t="inlineStr">
+        <is>
+          <t>2021 Q1</t>
         </is>
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="2" t="inlineStr">
-        <is>
-          <t>Tier 1 Threshold</t>
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>23.53%</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>2021 Q3</t>
+          <t>Tier 2 Threshold</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>26.07%</t>
+      <c r="A164" s="2" t="inlineStr">
+        <is>
+          <t>2021 Q2</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="2" t="inlineStr">
-        <is>
-          <t>Tier 1 Threshold</t>
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>25.08%</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>2021 Q4</t>
+          <t>Tier 2 Threshold</t>
         </is>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>26.07%</t>
+      <c r="A168" s="2" t="inlineStr">
+        <is>
+          <t>2021 Q3</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>26.07%</t>
         </is>
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>Tier 2 Threshold</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>35.00%</t>
+      <c r="A170" s="2" t="inlineStr">
+        <is>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>2022 Q1</t>
+          <t>Tier 2 Threshold</t>
         </is>
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>27.54%</t>
+      <c r="A172" s="2" t="inlineStr">
+        <is>
+          <t>2021 Q4</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>30.00%</t>
+          <t>26.07%</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
           <t>35.00%</t>
         </is>
       </c>
-    </row>
-    <row r="175">
-      <c r="A175" s="2" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" s="2" t="inlineStr">
         <is>
-          <t>Back Book Near Prime Cumulative Defaults</t>
+          <t>2022 Q1</t>
         </is>
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="2" t="inlineStr">
-        <is>
-          <t>Cohort</t>
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>27.54%</t>
         </is>
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="2" t="inlineStr">
-        <is>
-          <t>2018 Q1</t>
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Tier 1 Threshold</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>30.00%</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Tier 2 Threshold</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>4.24%</t>
+          <t>35.00%</t>
         </is>
       </c>
     </row>
     <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>Tier 1 Threshold</t>
-        </is>
-      </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>14.00%</t>
-        </is>
-      </c>
+      <c r="A180" s="2" t="inlineStr"/>
     </row>
     <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>Tier 2 Threshold</t>
-        </is>
-      </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>17.00%</t>
+      <c r="A181" s="2" t="inlineStr">
+        <is>
+          <t>Back Book Near Prime Cumulative Defaults</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>2018 Q2</t>
+          <t>Cohort</t>
         </is>
       </c>
     </row>
     <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>7.18%</t>
+      <c r="A183" s="2" t="inlineStr">
+        <is>
+          <t>2018 Q1</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>14.00%</t>
+          <t>4.24%</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
+          <t>14.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
           <t>17.00%</t>
         </is>
       </c>
     </row>
-    <row r="186">
-      <c r="A186" s="2" t="inlineStr">
-        <is>
-          <t>2018 H2</t>
-        </is>
-      </c>
-    </row>
     <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>9.72%</t>
+      <c r="A187" s="2" t="inlineStr">
+        <is>
+          <t>2018 Q2</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>14.00%</t>
+          <t>7.18%</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
+          <t>14.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
           <t>17.00%</t>
         </is>
       </c>
     </row>
-    <row r="190">
-      <c r="A190" s="2" t="inlineStr">
-        <is>
-          <t>2019 Q1</t>
-        </is>
-      </c>
-    </row>
     <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>9.21%</t>
+      <c r="A191" s="2" t="inlineStr">
+        <is>
+          <t>2018 H2</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>14.00%</t>
+          <t>9.72%</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
+          <t>14.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
           <t>17.00%</t>
         </is>
       </c>
     </row>
-    <row r="194">
-      <c r="A194" s="2" t="inlineStr">
-        <is>
-          <t>2019 Q2</t>
-        </is>
-      </c>
-    </row>
     <row r="195">
-      <c r="A195" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B195" t="inlineStr">
-        <is>
-          <t>9.12%</t>
+      <c r="A195" s="2" t="inlineStr">
+        <is>
+          <t>2019 Q1</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>14.00%</t>
+          <t>9.21%</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
+          <t>14.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
           <t>17.00%</t>
         </is>
       </c>
     </row>
-    <row r="198">
-      <c r="A198" s="2" t="inlineStr">
-        <is>
-          <t>2019 Q3</t>
-        </is>
-      </c>
-    </row>
     <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>9.06%</t>
+      <c r="A199" s="2" t="inlineStr">
+        <is>
+          <t>2019 Q2</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>14.00%</t>
+          <t>9.12%</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
+          <t>14.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
           <t>17.00%</t>
         </is>
       </c>
     </row>
-    <row r="202">
-      <c r="A202" s="2" t="inlineStr">
-        <is>
-          <t>2019 Q4</t>
-        </is>
-      </c>
-    </row>
     <row r="203">
-      <c r="A203" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B203" t="inlineStr">
-        <is>
-          <t>9.06%</t>
+      <c r="A203" s="2" t="inlineStr">
+        <is>
+          <t>2019 Q3</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>14.00%</t>
+          <t>9.06%</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
+          <t>14.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
           <t>17.00%</t>
         </is>
       </c>
     </row>
-    <row r="206">
-      <c r="A206" s="2" t="inlineStr">
+    <row r="207">
+      <c r="A207" s="2" t="inlineStr">
+        <is>
+          <t>2019 Q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>9.06%</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Tier 1 Threshold</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>14.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>17.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="2" t="inlineStr">
         <is>
           <t>2020 Q1</t>
-        </is>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>6.80%</t>
-        </is>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" s="2" t="inlineStr">
-        <is>
-          <t>Tier 1 Threshold</t>
-        </is>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" s="2" t="inlineStr">
-        <is>
-          <t>Tier 2 Threshold</t>
-        </is>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" s="2" t="inlineStr">
-        <is>
-          <t>2020 Q3-Q4 &amp; 2021 Vintages</t>
-        </is>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B211" t="inlineStr">
-        <is>
-          <t>13.72%</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>17.56%</t>
+          <t>6.80%</t>
         </is>
       </c>
     </row>
     <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>Tier 2 Threshold</t>
-        </is>
-      </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>18.85%</t>
+      <c r="A213" s="2" t="inlineStr">
+        <is>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="2" t="inlineStr"/>
+      <c r="A214" s="2" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>Front Book (Combined) Cumulative Defaults</t>
+          <t>2020 Q3-Q4 &amp; 2021 Vintages</t>
         </is>
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="2" t="inlineStr">
-        <is>
-          <t>Cohort</t>
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>13.72%</t>
         </is>
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="2" t="inlineStr">
-        <is>
-          <t>2022 Q1</t>
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Tier 1 Threshold</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>17.56%</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Actuals</t>
+          <t>Tier 2 Threshold</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>20.03%</t>
+          <t>18.85%</t>
         </is>
       </c>
     </row>
     <row r="219">
-      <c r="A219" t="inlineStr">
-        <is>
-          <t>Tier 1 Threshold</t>
-        </is>
-      </c>
-      <c r="B219" t="inlineStr">
-        <is>
-          <t>28.40%</t>
-        </is>
-      </c>
+      <c r="A219" s="2" t="inlineStr"/>
     </row>
     <row r="220">
-      <c r="A220" t="inlineStr">
-        <is>
-          <t>Tier 2 Threshold</t>
-        </is>
-      </c>
-      <c r="B220" t="inlineStr">
-        <is>
-          <t>33.10%</t>
+      <c r="A220" s="2" t="inlineStr">
+        <is>
+          <t>Front Book (Combined) Cumulative Defaults</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>2022 Q2</t>
+          <t>Cohort</t>
         </is>
       </c>
     </row>
     <row r="222">
-      <c r="A222" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B222" t="inlineStr">
-        <is>
-          <t>21.55%</t>
+      <c r="A222" s="2" t="inlineStr">
+        <is>
+          <t>2022 Q1</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>28.30%</t>
+          <t>20.03%</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
+          <t>28.40%</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
           <t>33.10%</t>
         </is>
       </c>
     </row>
-    <row r="225">
-      <c r="A225" s="2" t="inlineStr">
-        <is>
-          <t>2022 Q3</t>
-        </is>
-      </c>
-    </row>
     <row r="226">
-      <c r="A226" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>21.64%</t>
+      <c r="A226" s="2" t="inlineStr">
+        <is>
+          <t>2022 Q2</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>28.20%</t>
+          <t>21.55%</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>33.00%</t>
+          <t>28.30%</t>
         </is>
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="2" t="inlineStr">
-        <is>
-          <t>2022 Q4</t>
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>33.10%</t>
         </is>
       </c>
     </row>
     <row r="230">
-      <c r="A230" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B230" t="inlineStr">
-        <is>
-          <t>20.84%</t>
+      <c r="A230" s="2" t="inlineStr">
+        <is>
+          <t>2022 Q3</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>27.80%</t>
+          <t>21.64%</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>32.40%</t>
+          <t>28.20%</t>
         </is>
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="2" t="inlineStr">
-        <is>
-          <t>2023 Q1</t>
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>33.00%</t>
         </is>
       </c>
     </row>
     <row r="234">
-      <c r="A234" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B234" t="inlineStr">
-        <is>
-          <t>19.38%</t>
+      <c r="A234" s="2" t="inlineStr">
+        <is>
+          <t>2022 Q4</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>26.90%</t>
+          <t>20.84%</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>31.40%</t>
+          <t>27.80%</t>
         </is>
       </c>
     </row>
     <row r="237">
-      <c r="A237" s="2" t="inlineStr">
-        <is>
-          <t>2023 Q2</t>
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>32.40%</t>
         </is>
       </c>
     </row>
     <row r="238">
-      <c r="A238" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B238" t="inlineStr">
-        <is>
-          <t>18.49%</t>
+      <c r="A238" s="2" t="inlineStr">
+        <is>
+          <t>2023 Q1</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>25.50%</t>
+          <t>19.38%</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>29.70%</t>
+          <t>26.90%</t>
         </is>
       </c>
     </row>
     <row r="241">
-      <c r="A241" s="2" t="inlineStr">
-        <is>
-          <t>2023 Q3</t>
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>31.40%</t>
         </is>
       </c>
     </row>
     <row r="242">
-      <c r="A242" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B242" t="inlineStr">
-        <is>
-          <t>17.10%</t>
+      <c r="A242" s="2" t="inlineStr">
+        <is>
+          <t>2023 Q2</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Tier 1 Threshold</t>
+          <t>Actuals</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>23.60%</t>
+          <t>18.49%</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Tier 2 Threshold</t>
+          <t>Tier 1 Threshold</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
+        <is>
+          <t>25.50%</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>29.70%</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="2" t="inlineStr">
+        <is>
+          <t>2023 Q3</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>17.10%</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Tier 1 Threshold</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>23.60%</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Tier 2 Threshold</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
         <is>
           <t>27.60%</t>
         </is>

</xml_diff>

<commit_message>
password changes for salary finance
</commit_message>
<xml_diff>
--- a/oakbrook_monitoring_sheet.xlsx
+++ b/oakbrook_monitoring_sheet.xlsx
@@ -439,7 +439,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>21070930.15</v>
+        <v>23589205.05</v>
       </c>
     </row>
     <row r="3">
@@ -449,7 +449,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11595540.13</v>
+        <v>12798874.58</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9475390.02</v>
+        <v>10790330.47</v>
       </c>
     </row>
     <row r="5">
@@ -479,7 +479,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>221226131.89</v>
+        <v>226329478.62</v>
       </c>
     </row>
     <row r="8">
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>105483833.65</v>
+        <v>106835116.29</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>115742298.24</v>
+        <v>119494362.33</v>
       </c>
     </row>
     <row r="10">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>81931853.2871497</v>
+        <v>82930332.0071497</v>
       </c>
     </row>
     <row r="14">
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>94145067.68999998</v>
+        <v>97955830.00999998</v>
       </c>
     </row>
     <row r="21">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>16152826.51</v>
+        <v>16500000</v>
       </c>
     </row>
     <row r="22">
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>38.33208030009099</v>
+        <v>38.36175787029699</v>
       </c>
     </row>
     <row r="25">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>54.13101567882766</v>
+        <v>54.5910283895756</v>
       </c>
     </row>
     <row r="26">
@@ -636,7 +636,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>23.9334352353275</v>
+        <v>23.85181807547456</v>
       </c>
     </row>
     <row r="27">
@@ -685,13 +685,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Actuals</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>4490320.699999999</v>
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>Actuals</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -726,7 +723,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>28.93%</t>
+          <t>29.67%</t>
         </is>
       </c>
     </row>
@@ -764,7 +761,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>24.61%</t>
+          <t>24.90%</t>
         </is>
       </c>
     </row>
@@ -783,7 +780,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>3.14%</t>
+          <t>3.26%</t>
         </is>
       </c>
     </row>
@@ -818,7 +815,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>28.72321441505379</v>
+        <v>28.56709602348285</v>
       </c>
     </row>
     <row r="50">
@@ -845,7 +842,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>732.0672473061538</v>
+        <v>730.4072408515789</v>
       </c>
     </row>
     <row r="53">
@@ -872,7 +869,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>2256.685180824217</v>
+        <v>2260.582755498804</v>
       </c>
     </row>
     <row r="56">
@@ -907,7 +904,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>5.43%</t>
+          <t>5.12%</t>
         </is>
       </c>
     </row>
@@ -938,7 +935,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>12.50%</t>
+          <t>11.90%</t>
         </is>
       </c>
     </row>
@@ -969,7 +966,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>4.05%</t>
+          <t>3.73%</t>
         </is>
       </c>
     </row>
@@ -1000,7 +997,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>4.52%</t>
+          <t>4.33%</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1028,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>12.37%</t>
+          <t>12.89%</t>
         </is>
       </c>
     </row>
@@ -1062,7 +1059,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>3.50%</t>
+          <t>3.20%</t>
         </is>
       </c>
     </row>
@@ -1186,7 +1183,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>0.02%</t>
+          <t>0.03%</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2124,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>27.60%</t>
+          <t>27.61%</t>
         </is>
       </c>
     </row>
@@ -2531,7 +2528,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>11.92%</t>
+          <t>11.25%</t>
         </is>
       </c>
     </row>
@@ -2591,7 +2588,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>20.18%</t>
+          <t>20.23%</t>
         </is>
       </c>
     </row>
@@ -2634,7 +2631,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>21.72%</t>
+          <t>21.80%</t>
         </is>
       </c>
     </row>
@@ -2658,7 +2655,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>33.10%</t>
+          <t>33.20%</t>
         </is>
       </c>
     </row>
@@ -2677,7 +2674,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>21.97%</t>
+          <t>22.01%</t>
         </is>
       </c>
     </row>
@@ -2720,7 +2717,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>21.17%</t>
+          <t>21.24%</t>
         </is>
       </c>
     </row>
@@ -2763,7 +2760,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>20.06%</t>
+          <t>20.20%</t>
         </is>
       </c>
     </row>
@@ -2806,7 +2803,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>19.27%</t>
+          <t>19.50%</t>
         </is>
       </c>
     </row>
@@ -2818,7 +2815,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>26.90%</t>
+          <t>27.20%</t>
         </is>
       </c>
     </row>
@@ -2830,7 +2827,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>31.40%</t>
+          <t>31.80%</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2846,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>18.22%</t>
+          <t>18.54%</t>
         </is>
       </c>
     </row>
@@ -2861,7 +2858,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>25.50%</t>
+          <t>26.10%</t>
         </is>
       </c>
     </row>
@@ -2873,7 +2870,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>29.70%</t>
+          <t>30.50%</t>
         </is>
       </c>
     </row>

</xml_diff>